<commit_message>
Improve test file for detecting TimeSpan type cell.
The test files checked only predefined formats 21. The predefined formats 18-20 and 45-47 were added to the test file.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/TryToLoad/CellsWithTimeSpanDataTypeOrFormatting.xlsx
+++ b/ClosedXML.Tests/Resource/TryToLoad/CellsWithTimeSpanDataTypeOrFormatting.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43A7AB93-398E-469F-88BF-276AABBEC2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\havli\source\repos\ClosedXML\ClosedXML.Tests\Resource\TryToLoad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F10E258-C934-432F-87BD-248816DB07DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Format</t>
   </si>
@@ -42,9 +47,6 @@
     <t>Raw Value</t>
   </si>
   <si>
-    <t>Custom hh:mm:ss</t>
-  </si>
-  <si>
     <t>Time *1:30:55 PM (US)</t>
   </si>
   <si>
@@ -55,6 +57,27 @@
   </si>
   <si>
     <t>Time 30:55.2 (US)</t>
+  </si>
+  <si>
+    <t>Time fmt 21: h:mm:ss</t>
+  </si>
+  <si>
+    <t>Time fmt 20: H:mm</t>
+  </si>
+  <si>
+    <t>Time fmt 19: h:mm:ss tt</t>
+  </si>
+  <si>
+    <t>Time fmt 18: h:mm tt</t>
+  </si>
+  <si>
+    <t>Time fmt 45: mm:ss</t>
+  </si>
+  <si>
+    <t>Time fmt 46: [h]:mm:ss</t>
+  </si>
+  <si>
+    <t>Time fmt 47: mm:ss.0</t>
   </si>
 </sst>
 </file>
@@ -68,7 +91,7 @@
     <numFmt numFmtId="167" formatCode="mm:ss.0;@"/>
     <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -114,6 +137,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,20 +457,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -452,11 +481,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8">
         <v>0.56313888888888886</v>
       </c>
       <c r="C2" s="7">
@@ -464,55 +493,128 @@
         <v>0.56313888888888886</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C3" s="7">
+        <f>B3</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C4" s="7">
+        <f>B4</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C5" s="7">
+        <f>B5</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C6" s="7">
+        <f>B6</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C8" s="7">
+        <f>B8</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:C12" si="0">B9</f>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.56313888888888886</v>
-      </c>
-      <c r="C3" s="7">
-        <f t="shared" ref="C3:C6" si="0">B3</f>
-        <v>0.56313888888888886</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="B10" s="4">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.56313888888888886</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.56313888888888886</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B11" s="3">
+        <v>0.56313888888888886</v>
+      </c>
+      <c r="C11" s="7">
         <f t="shared" si="0"/>
         <v>0.56313888888888886</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.56313888888888886</v>
-      </c>
-      <c r="C5" s="7">
-        <f t="shared" si="0"/>
-        <v>0.56313888888888886</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="B12" s="6">
         <v>2.1472222222222222E-2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>2.1472222222222222E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>